<commit_message>
Fix calculation approach for mid rises and mid falls
Updated the calculation logic for mid rises and mid falls to ensure accuracy in rise percentage and event data. Adjusted related output files and scripts accordingly.

- Corrected mid rise and mid fall percentage calculations in JSON files
- Updated `bsfc_rise_volatility_analysis.json` with revised rise event data
- Modified `backtest_insider_conviction_strategy.py` to align with new calculation logic
- Added `bsfc_insider_conviction_poc.json` for insider conviction analysis
- Updated XLSX files for BSFC and GROV rise events with recalculated data

============================================================
  FEATURE LABELS
============================================================

# POC_tests
</commit_message>
<xml_diff>
--- a/output CSVs/bsfc_rise_events.xlsx
+++ b/output CSVs/bsfc_rise_events.xlsx
@@ -517,7 +517,7 @@
         <v>34</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>23.81</v>
+        <v>12.76</v>
       </c>
       <c r="F2" s="2" t="inlineStr">
         <is>
@@ -525,7 +525,7 @@
         </is>
       </c>
       <c r="G2" s="2" t="n">
-        <v>23.81</v>
+        <v>12.76</v>
       </c>
       <c r="H2" s="2" t="n"/>
     </row>
@@ -549,15 +549,15 @@
         <v>204</v>
       </c>
       <c r="E3" s="3" t="n">
-        <v>-23.08</v>
+        <v>-10.25</v>
       </c>
       <c r="F3" s="3" t="inlineStr">
         <is>
-          <t>31/42</t>
+          <t>37/42</t>
         </is>
       </c>
       <c r="G3" s="3" t="n">
-        <v>0.73</v>
+        <v>2.51</v>
       </c>
       <c r="H3" s="3" t="n"/>
     </row>
@@ -581,15 +581,15 @@
         <v>35</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>15</v>
+        <v>-44.83</v>
       </c>
       <c r="F4" s="2" t="inlineStr">
         <is>
-          <t>30/43</t>
+          <t>7/43</t>
         </is>
       </c>
       <c r="G4" s="2" t="n">
-        <v>15.73</v>
+        <v>-42.33</v>
       </c>
       <c r="H4" s="2" t="n"/>
     </row>
@@ -613,7 +613,7 @@
         <v>4</v>
       </c>
       <c r="E5" s="3" t="n">
-        <v>-56.09</v>
+        <v>56.78</v>
       </c>
       <c r="F5" s="3" t="inlineStr">
         <is>
@@ -621,7 +621,7 @@
         </is>
       </c>
       <c r="G5" s="3" t="n">
-        <v>-40.35</v>
+        <v>14.46</v>
       </c>
       <c r="H5" s="3" t="n"/>
     </row>
@@ -645,15 +645,15 @@
         <v>9</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>122.77</v>
+        <v>106.58</v>
       </c>
       <c r="F6" s="2" t="inlineStr">
         <is>
-          <t>4/43</t>
+          <t>1/43</t>
         </is>
       </c>
       <c r="G6" s="2" t="n">
-        <v>82.42</v>
+        <v>121.04</v>
       </c>
       <c r="H6" s="2" t="n"/>
     </row>
@@ -677,7 +677,7 @@
         <v>41</v>
       </c>
       <c r="E7" s="3" t="n">
-        <v>-15.56</v>
+        <v>8.58</v>
       </c>
       <c r="F7" s="3" t="inlineStr">
         <is>
@@ -685,7 +685,7 @@
         </is>
       </c>
       <c r="G7" s="3" t="n">
-        <v>66.86</v>
+        <v>129.62</v>
       </c>
       <c r="H7" s="3" t="n"/>
     </row>
@@ -709,15 +709,15 @@
         <v>19</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>163.11</v>
+        <v>88.90000000000001</v>
       </c>
       <c r="F8" s="2" t="inlineStr">
         <is>
-          <t>1/43</t>
+          <t>2/43</t>
         </is>
       </c>
       <c r="G8" s="2" t="n">
-        <v>229.97</v>
+        <v>218.53</v>
       </c>
       <c r="H8" s="2" t="n"/>
     </row>
@@ -741,15 +741,15 @@
         <v>13</v>
       </c>
       <c r="E9" s="3" t="n">
-        <v>-24.66</v>
+        <v>-6.5</v>
       </c>
       <c r="F9" s="3" t="inlineStr">
         <is>
-          <t>30/42</t>
+          <t>40/42</t>
         </is>
       </c>
       <c r="G9" s="3" t="n">
-        <v>205.31</v>
+        <v>212.03</v>
       </c>
       <c r="H9" s="3" t="n"/>
     </row>
@@ -773,15 +773,15 @@
         <v>142</v>
       </c>
       <c r="E10" s="2" t="n">
-        <v>41.6</v>
+        <v>62.14</v>
       </c>
       <c r="F10" s="2" t="inlineStr">
         <is>
-          <t>11/43</t>
+          <t>4/43</t>
         </is>
       </c>
       <c r="G10" s="2" t="n">
-        <v>246.91</v>
+        <v>274.17</v>
       </c>
       <c r="H10" s="2" t="inlineStr">
         <is>
@@ -809,15 +809,15 @@
         <v>14</v>
       </c>
       <c r="E11" s="3" t="n">
-        <v>-16</v>
+        <v>-3.45</v>
       </c>
       <c r="F11" s="3" t="inlineStr">
         <is>
-          <t>36/42</t>
+          <t>42/42</t>
         </is>
       </c>
       <c r="G11" s="3" t="n">
-        <v>230.91</v>
+        <v>270.72</v>
       </c>
       <c r="H11" s="3" t="n"/>
     </row>
@@ -841,15 +841,15 @@
         <v>20</v>
       </c>
       <c r="E12" s="2" t="n">
-        <v>24.92</v>
+        <v>-12.39</v>
       </c>
       <c r="F12" s="2" t="inlineStr">
         <is>
-          <t>22/43</t>
+          <t>25/43</t>
         </is>
       </c>
       <c r="G12" s="2" t="n">
-        <v>255.83</v>
+        <v>258.33</v>
       </c>
       <c r="H12" s="2" t="n"/>
     </row>
@@ -873,15 +873,15 @@
         <v>24</v>
       </c>
       <c r="E13" s="3" t="n">
-        <v>-65.37</v>
+        <v>-88.48999999999999</v>
       </c>
       <c r="F13" s="3" t="inlineStr">
         <is>
-          <t>5/42</t>
+          <t>2/42</t>
         </is>
       </c>
       <c r="G13" s="3" t="n">
-        <v>190.46</v>
+        <v>169.84</v>
       </c>
       <c r="H13" s="3" t="inlineStr">
         <is>
@@ -909,15 +909,15 @@
         <v>22</v>
       </c>
       <c r="E14" s="2" t="n">
-        <v>33.94</v>
+        <v>-29.53</v>
       </c>
       <c r="F14" s="2" t="inlineStr">
         <is>
-          <t>19/43</t>
+          <t>11/43</t>
         </is>
       </c>
       <c r="G14" s="2" t="n">
-        <v>224.4</v>
+        <v>140.31</v>
       </c>
       <c r="H14" s="2" t="n"/>
     </row>
@@ -941,15 +941,15 @@
         <v>35</v>
       </c>
       <c r="E15" s="3" t="n">
-        <v>-56.71</v>
+        <v>-42.53</v>
       </c>
       <c r="F15" s="3" t="inlineStr">
         <is>
-          <t>9/42</t>
+          <t>18/42</t>
         </is>
       </c>
       <c r="G15" s="3" t="n">
-        <v>167.69</v>
+        <v>97.78</v>
       </c>
       <c r="H15" s="3" t="n"/>
     </row>
@@ -973,7 +973,7 @@
         <v>6</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>131.43</v>
+        <v>71.69</v>
       </c>
       <c r="F16" s="2" t="inlineStr">
         <is>
@@ -981,7 +981,7 @@
         </is>
       </c>
       <c r="G16" s="2" t="n">
-        <v>299.12</v>
+        <v>169.47</v>
       </c>
       <c r="H16" s="2" t="n"/>
     </row>
@@ -1005,7 +1005,7 @@
         <v>35</v>
       </c>
       <c r="E17" s="3" t="n">
-        <v>-60.49</v>
+        <v>-64.65000000000001</v>
       </c>
       <c r="F17" s="3" t="inlineStr">
         <is>
@@ -1013,7 +1013,7 @@
         </is>
       </c>
       <c r="G17" s="3" t="n">
-        <v>238.63</v>
+        <v>104.83</v>
       </c>
       <c r="H17" s="3" t="inlineStr">
         <is>
@@ -1041,15 +1041,15 @@
         <v>27</v>
       </c>
       <c r="E18" s="2" t="n">
-        <v>52.98</v>
+        <v>27.29</v>
       </c>
       <c r="F18" s="2" t="inlineStr">
         <is>
-          <t>9/43</t>
+          <t>14/43</t>
         </is>
       </c>
       <c r="G18" s="2" t="n">
-        <v>291.6</v>
+        <v>132.12</v>
       </c>
       <c r="H18" s="2" t="n"/>
     </row>
@@ -1073,15 +1073,15 @@
         <v>18</v>
       </c>
       <c r="E19" s="3" t="n">
-        <v>-41.63</v>
+        <v>-48.7</v>
       </c>
       <c r="F19" s="3" t="inlineStr">
         <is>
-          <t>18/42</t>
+          <t>14/42</t>
         </is>
       </c>
       <c r="G19" s="3" t="n">
-        <v>249.97</v>
+        <v>83.42</v>
       </c>
       <c r="H19" s="3" t="n"/>
     </row>
@@ -1105,15 +1105,15 @@
         <v>3</v>
       </c>
       <c r="E20" s="2" t="n">
-        <v>6.67</v>
+        <v>1.34</v>
       </c>
       <c r="F20" s="2" t="inlineStr">
         <is>
-          <t>40/43</t>
+          <t>42/43</t>
         </is>
       </c>
       <c r="G20" s="2" t="n">
-        <v>256.63</v>
+        <v>84.76000000000001</v>
       </c>
       <c r="H20" s="2" t="n"/>
     </row>
@@ -1137,15 +1137,15 @@
         <v>20</v>
       </c>
       <c r="E21" s="3" t="n">
-        <v>-29.38</v>
+        <v>-32.76</v>
       </c>
       <c r="F21" s="3" t="inlineStr">
         <is>
-          <t>27/42</t>
+          <t>20/42</t>
         </is>
       </c>
       <c r="G21" s="3" t="n">
-        <v>227.26</v>
+        <v>52</v>
       </c>
       <c r="H21" s="3" t="n"/>
     </row>
@@ -1169,15 +1169,15 @@
         <v>28</v>
       </c>
       <c r="E22" s="2" t="n">
-        <v>40.71</v>
+        <v>25.27</v>
       </c>
       <c r="F22" s="2" t="inlineStr">
         <is>
-          <t>13/43</t>
+          <t>17/43</t>
         </is>
       </c>
       <c r="G22" s="2" t="n">
-        <v>267.97</v>
+        <v>77.28</v>
       </c>
       <c r="H22" s="2" t="n"/>
     </row>
@@ -1201,15 +1201,15 @@
         <v>12</v>
       </c>
       <c r="E23" s="3" t="n">
-        <v>-32.08</v>
+        <v>-25.35</v>
       </c>
       <c r="F23" s="3" t="inlineStr">
         <is>
-          <t>23/42</t>
+          <t>24/42</t>
         </is>
       </c>
       <c r="G23" s="3" t="n">
-        <v>235.89</v>
+        <v>51.92</v>
       </c>
       <c r="H23" s="3" t="n"/>
     </row>
@@ -1233,15 +1233,15 @@
         <v>2</v>
       </c>
       <c r="E24" s="2" t="n">
-        <v>37.04</v>
+        <v>26.46</v>
       </c>
       <c r="F24" s="2" t="inlineStr">
         <is>
-          <t>17/43</t>
+          <t>16/43</t>
         </is>
       </c>
       <c r="G24" s="2" t="n">
-        <v>272.93</v>
+        <v>78.38</v>
       </c>
       <c r="H24" s="2" t="n"/>
     </row>
@@ -1265,15 +1265,15 @@
         <v>36</v>
       </c>
       <c r="E25" s="3" t="n">
-        <v>-15.54</v>
+        <v>-14.26</v>
       </c>
       <c r="F25" s="3" t="inlineStr">
         <is>
-          <t>40/42</t>
+          <t>34/42</t>
         </is>
       </c>
       <c r="G25" s="3" t="n">
-        <v>257.39</v>
+        <v>64.12</v>
       </c>
       <c r="H25" s="3" t="n"/>
     </row>
@@ -1297,15 +1297,15 @@
         <v>13</v>
       </c>
       <c r="E26" s="2" t="n">
-        <v>10.4</v>
+        <v>3.24</v>
       </c>
       <c r="F26" s="2" t="inlineStr">
         <is>
-          <t>35/43</t>
+          <t>38/43</t>
         </is>
       </c>
       <c r="G26" s="2" t="n">
-        <v>267.79</v>
+        <v>67.36</v>
       </c>
       <c r="H26" s="2" t="n"/>
     </row>
@@ -1329,7 +1329,7 @@
         <v>36</v>
       </c>
       <c r="E27" s="3" t="n">
-        <v>-45.07</v>
+        <v>-48.41</v>
       </c>
       <c r="F27" s="3" t="inlineStr">
         <is>
@@ -1337,7 +1337,7 @@
         </is>
       </c>
       <c r="G27" s="3" t="n">
-        <v>222.72</v>
+        <v>18.95</v>
       </c>
       <c r="H27" s="3" t="n"/>
     </row>
@@ -1361,15 +1361,15 @@
         <v>14</v>
       </c>
       <c r="E28" s="2" t="n">
-        <v>33.25</v>
+        <v>26.58</v>
       </c>
       <c r="F28" s="2" t="inlineStr">
         <is>
-          <t>20/43</t>
+          <t>15/43</t>
         </is>
       </c>
       <c r="G28" s="2" t="n">
-        <v>255.96</v>
+        <v>45.53</v>
       </c>
       <c r="H28" s="2" t="inlineStr">
         <is>
@@ -1397,7 +1397,7 @@
         <v>18</v>
       </c>
       <c r="E29" s="3" t="n">
-        <v>-12.87</v>
+        <v>-4.82</v>
       </c>
       <c r="F29" s="3" t="inlineStr">
         <is>
@@ -1405,7 +1405,7 @@
         </is>
       </c>
       <c r="G29" s="3" t="n">
-        <v>243.09</v>
+        <v>40.71</v>
       </c>
       <c r="H29" s="3" t="n"/>
     </row>
@@ -1429,15 +1429,15 @@
         <v>3</v>
       </c>
       <c r="E30" s="2" t="n">
-        <v>8.99</v>
+        <v>6.24</v>
       </c>
       <c r="F30" s="2" t="inlineStr">
         <is>
-          <t>37/43</t>
+          <t>32/43</t>
         </is>
       </c>
       <c r="G30" s="2" t="n">
-        <v>252.08</v>
+        <v>46.95</v>
       </c>
       <c r="H30" s="2" t="inlineStr">
         <is>
@@ -1465,15 +1465,15 @@
         <v>45</v>
       </c>
       <c r="E31" s="3" t="n">
-        <v>-53.61</v>
+        <v>-71.22</v>
       </c>
       <c r="F31" s="3" t="inlineStr">
         <is>
-          <t>11/42</t>
+          <t>5/42</t>
         </is>
       </c>
       <c r="G31" s="3" t="n">
-        <v>198.47</v>
+        <v>-24.27</v>
       </c>
       <c r="H31" s="3" t="n"/>
     </row>
@@ -1497,15 +1497,15 @@
         <v>3</v>
       </c>
       <c r="E32" s="2" t="n">
-        <v>8.890000000000001</v>
+        <v>6.14</v>
       </c>
       <c r="F32" s="2" t="inlineStr">
         <is>
-          <t>38/43</t>
+          <t>33/43</t>
         </is>
       </c>
       <c r="G32" s="2" t="n">
-        <v>207.36</v>
+        <v>-18.12</v>
       </c>
       <c r="H32" s="2" t="n"/>
     </row>
@@ -1529,15 +1529,15 @@
         <v>13</v>
       </c>
       <c r="E33" s="3" t="n">
-        <v>-28.57</v>
+        <v>-17.62</v>
       </c>
       <c r="F33" s="3" t="inlineStr">
         <is>
-          <t>28/42</t>
+          <t>30/42</t>
         </is>
       </c>
       <c r="G33" s="3" t="n">
-        <v>178.79</v>
+        <v>-35.75</v>
       </c>
       <c r="H33" s="3" t="n"/>
     </row>
@@ -1561,15 +1561,15 @@
         <v>8</v>
       </c>
       <c r="E34" s="2" t="n">
-        <v>37.14</v>
+        <v>29.99</v>
       </c>
       <c r="F34" s="2" t="inlineStr">
         <is>
-          <t>16/43</t>
+          <t>10/43</t>
         </is>
       </c>
       <c r="G34" s="2" t="n">
-        <v>215.93</v>
+        <v>-5.76</v>
       </c>
       <c r="H34" s="2" t="n"/>
     </row>
@@ -1593,15 +1593,15 @@
         <v>17</v>
       </c>
       <c r="E35" s="3" t="n">
-        <v>-31.46</v>
+        <v>-24.2</v>
       </c>
       <c r="F35" s="3" t="inlineStr">
         <is>
-          <t>24/42</t>
+          <t>25/42</t>
         </is>
       </c>
       <c r="G35" s="3" t="n">
-        <v>184.47</v>
+        <v>-29.96</v>
       </c>
       <c r="H35" s="3" t="n"/>
     </row>
@@ -1625,15 +1625,15 @@
         <v>5</v>
       </c>
       <c r="E36" s="2" t="n">
-        <v>58.05</v>
+        <v>-20.19</v>
       </c>
       <c r="F36" s="2" t="inlineStr">
         <is>
-          <t>8/43</t>
+          <t>19/43</t>
         </is>
       </c>
       <c r="G36" s="2" t="n">
-        <v>242.53</v>
+        <v>-50.15</v>
       </c>
       <c r="H36" s="2" t="n"/>
     </row>
@@ -1657,15 +1657,15 @@
         <v>13</v>
       </c>
       <c r="E37" s="3" t="n">
-        <v>-67.31</v>
+        <v>-66.84999999999999</v>
       </c>
       <c r="F37" s="3" t="inlineStr">
         <is>
-          <t>4/42</t>
+          <t>6/42</t>
         </is>
       </c>
       <c r="G37" s="3" t="n">
-        <v>175.22</v>
+        <v>-117</v>
       </c>
       <c r="H37" s="3" t="n"/>
     </row>
@@ -1689,15 +1689,15 @@
         <v>2</v>
       </c>
       <c r="E38" s="2" t="n">
-        <v>12.94</v>
+        <v>-9.640000000000001</v>
       </c>
       <c r="F38" s="2" t="inlineStr">
         <is>
-          <t>33/43</t>
+          <t>29/43</t>
         </is>
       </c>
       <c r="G38" s="2" t="n">
-        <v>188.16</v>
+        <v>-126.64</v>
       </c>
       <c r="H38" s="2" t="n"/>
     </row>
@@ -1721,15 +1721,15 @@
         <v>11</v>
       </c>
       <c r="E39" s="3" t="n">
-        <v>-20.31</v>
+        <v>-13.78</v>
       </c>
       <c r="F39" s="3" t="inlineStr">
         <is>
-          <t>33/42</t>
+          <t>35/42</t>
         </is>
       </c>
       <c r="G39" s="3" t="n">
-        <v>167.85</v>
+        <v>-140.41</v>
       </c>
       <c r="H39" s="3" t="n"/>
     </row>
@@ -1753,15 +1753,15 @@
         <v>7</v>
       </c>
       <c r="E40" s="2" t="n">
-        <v>37.25</v>
+        <v>13.97</v>
       </c>
       <c r="F40" s="2" t="inlineStr">
         <is>
-          <t>15/43</t>
+          <t>21/43</t>
         </is>
       </c>
       <c r="G40" s="2" t="n">
-        <v>205.1</v>
+        <v>-126.44</v>
       </c>
       <c r="H40" s="2" t="n"/>
     </row>
@@ -1785,15 +1785,15 @@
         <v>8</v>
       </c>
       <c r="E41" s="3" t="n">
-        <v>-38.1</v>
+        <v>-21.85</v>
       </c>
       <c r="F41" s="3" t="inlineStr">
         <is>
-          <t>21/42</t>
+          <t>28/42</t>
         </is>
       </c>
       <c r="G41" s="3" t="n">
-        <v>167.01</v>
+        <v>-148.29</v>
       </c>
       <c r="H41" s="3" t="n"/>
     </row>
@@ -1817,15 +1817,15 @@
         <v>4</v>
       </c>
       <c r="E42" s="2" t="n">
-        <v>36.15</v>
+        <v>27.52</v>
       </c>
       <c r="F42" s="2" t="inlineStr">
         <is>
-          <t>18/43</t>
+          <t>13/43</t>
         </is>
       </c>
       <c r="G42" s="2" t="n">
-        <v>203.16</v>
+        <v>-120.77</v>
       </c>
       <c r="H42" s="2" t="n"/>
     </row>
@@ -1849,15 +1849,15 @@
         <v>13</v>
       </c>
       <c r="E43" s="3" t="n">
-        <v>-29.38</v>
+        <v>-28.35</v>
       </c>
       <c r="F43" s="3" t="inlineStr">
         <is>
-          <t>26/42</t>
+          <t>22/42</t>
         </is>
       </c>
       <c r="G43" s="3" t="n">
-        <v>173.78</v>
+        <v>-149.12</v>
       </c>
       <c r="H43" s="3" t="n"/>
     </row>
@@ -1881,15 +1881,15 @@
         <v>9</v>
       </c>
       <c r="E44" s="2" t="n">
-        <v>16</v>
+        <v>8.640000000000001</v>
       </c>
       <c r="F44" s="2" t="inlineStr">
         <is>
-          <t>28/43</t>
+          <t>30/43</t>
         </is>
       </c>
       <c r="G44" s="2" t="n">
-        <v>189.78</v>
+        <v>-140.48</v>
       </c>
       <c r="H44" s="2" t="n"/>
     </row>
@@ -1913,15 +1913,15 @@
         <v>21</v>
       </c>
       <c r="E45" s="3" t="n">
-        <v>-22.07</v>
+        <v>-22.84</v>
       </c>
       <c r="F45" s="3" t="inlineStr">
         <is>
-          <t>32/42</t>
+          <t>27/42</t>
         </is>
       </c>
       <c r="G45" s="3" t="n">
-        <v>167.71</v>
+        <v>-163.32</v>
       </c>
       <c r="H45" s="3" t="n"/>
     </row>
@@ -1945,15 +1945,15 @@
         <v>12</v>
       </c>
       <c r="E46" s="2" t="n">
-        <v>11.5</v>
+        <v>-10.57</v>
       </c>
       <c r="F46" s="2" t="inlineStr">
         <is>
-          <t>34/43</t>
+          <t>28/43</t>
         </is>
       </c>
       <c r="G46" s="2" t="n">
-        <v>179.22</v>
+        <v>-173.89</v>
       </c>
       <c r="H46" s="2" t="n"/>
     </row>
@@ -1977,15 +1977,15 @@
         <v>48</v>
       </c>
       <c r="E47" s="3" t="n">
-        <v>-56.75</v>
+        <v>-71.22</v>
       </c>
       <c r="F47" s="3" t="inlineStr">
         <is>
-          <t>8/42</t>
+          <t>4/42</t>
         </is>
       </c>
       <c r="G47" s="3" t="n">
-        <v>122.47</v>
+        <v>-245.11</v>
       </c>
       <c r="H47" s="3" t="n"/>
     </row>
@@ -2009,15 +2009,15 @@
         <v>8</v>
       </c>
       <c r="E48" s="2" t="n">
-        <v>10.09</v>
+        <v>0.78</v>
       </c>
       <c r="F48" s="2" t="inlineStr">
         <is>
-          <t>36/43</t>
+          <t>43/43</t>
         </is>
       </c>
       <c r="G48" s="2" t="n">
-        <v>132.56</v>
+        <v>-244.33</v>
       </c>
       <c r="H48" s="2" t="n"/>
     </row>
@@ -2041,15 +2041,15 @@
         <v>17</v>
       </c>
       <c r="E49" s="3" t="n">
-        <v>-30.08</v>
+        <v>-30.6</v>
       </c>
       <c r="F49" s="3" t="inlineStr">
         <is>
-          <t>25/42</t>
+          <t>21/42</t>
         </is>
       </c>
       <c r="G49" s="3" t="n">
-        <v>102.48</v>
+        <v>-274.93</v>
       </c>
       <c r="H49" s="3" t="n"/>
     </row>
@@ -2073,15 +2073,15 @@
         <v>7</v>
       </c>
       <c r="E50" s="2" t="n">
-        <v>48.99</v>
+        <v>11.86</v>
       </c>
       <c r="F50" s="2" t="inlineStr">
         <is>
-          <t>10/43</t>
+          <t>26/43</t>
         </is>
       </c>
       <c r="G50" s="2" t="n">
-        <v>151.47</v>
+        <v>-263.06</v>
       </c>
       <c r="H50" s="2" t="n"/>
     </row>
@@ -2105,7 +2105,7 @@
         <v>50</v>
       </c>
       <c r="E51" s="3" t="n">
-        <v>-82.40000000000001</v>
+        <v>-142.02</v>
       </c>
       <c r="F51" s="3" t="inlineStr">
         <is>
@@ -2113,7 +2113,7 @@
         </is>
       </c>
       <c r="G51" s="3" t="n">
-        <v>69.06999999999999</v>
+        <v>-405.08</v>
       </c>
       <c r="H51" s="3" t="n"/>
     </row>
@@ -2137,7 +2137,7 @@
         <v>2</v>
       </c>
       <c r="E52" s="2" t="n">
-        <v>18.18</v>
+        <v>-11.4</v>
       </c>
       <c r="F52" s="2" t="inlineStr">
         <is>
@@ -2145,7 +2145,7 @@
         </is>
       </c>
       <c r="G52" s="2" t="n">
-        <v>87.25</v>
+        <v>-416.48</v>
       </c>
       <c r="H52" s="2" t="n"/>
     </row>
@@ -2169,15 +2169,15 @@
         <v>29</v>
       </c>
       <c r="E53" s="3" t="n">
-        <v>-51.54</v>
+        <v>-64.29000000000001</v>
       </c>
       <c r="F53" s="3" t="inlineStr">
         <is>
-          <t>12/42</t>
+          <t>8/42</t>
         </is>
       </c>
       <c r="G53" s="3" t="n">
-        <v>35.71</v>
+        <v>-480.77</v>
       </c>
       <c r="H53" s="3" t="n"/>
     </row>
@@ -2201,15 +2201,15 @@
         <v>23</v>
       </c>
       <c r="E54" s="2" t="n">
-        <v>41.27</v>
+        <v>30.93</v>
       </c>
       <c r="F54" s="2" t="inlineStr">
         <is>
-          <t>12/43</t>
+          <t>9/43</t>
         </is>
       </c>
       <c r="G54" s="2" t="n">
-        <v>76.98</v>
+        <v>-449.85</v>
       </c>
       <c r="H54" s="2" t="n"/>
     </row>
@@ -2233,15 +2233,15 @@
         <v>6</v>
       </c>
       <c r="E55" s="3" t="n">
-        <v>-17.98</v>
+        <v>-16.67</v>
       </c>
       <c r="F55" s="3" t="inlineStr">
         <is>
-          <t>35/42</t>
+          <t>31/42</t>
         </is>
       </c>
       <c r="G55" s="3" t="n">
-        <v>59</v>
+        <v>-466.52</v>
       </c>
       <c r="H55" s="3" t="n"/>
     </row>
@@ -2265,15 +2265,15 @@
         <v>12</v>
       </c>
       <c r="E56" s="2" t="n">
-        <v>13.7</v>
+        <v>5.41</v>
       </c>
       <c r="F56" s="2" t="inlineStr">
         <is>
-          <t>32/43</t>
+          <t>34/43</t>
         </is>
       </c>
       <c r="G56" s="2" t="n">
-        <v>72.7</v>
+        <v>-461.11</v>
       </c>
       <c r="H56" s="2" t="n"/>
     </row>
@@ -2297,15 +2297,15 @@
         <v>20</v>
       </c>
       <c r="E57" s="3" t="n">
-        <v>-15.66</v>
+        <v>-15.32</v>
       </c>
       <c r="F57" s="3" t="inlineStr">
         <is>
-          <t>37/42</t>
+          <t>33/42</t>
         </is>
       </c>
       <c r="G57" s="3" t="n">
-        <v>57.04</v>
+        <v>-476.43</v>
       </c>
       <c r="H57" s="3" t="inlineStr">
         <is>
@@ -2333,15 +2333,15 @@
         <v>15</v>
       </c>
       <c r="E58" s="2" t="n">
-        <v>19.29</v>
+        <v>5.22</v>
       </c>
       <c r="F58" s="2" t="inlineStr">
         <is>
-          <t>25/43</t>
+          <t>35/43</t>
         </is>
       </c>
       <c r="G58" s="2" t="n">
-        <v>76.33</v>
+        <v>-471.21</v>
       </c>
       <c r="H58" s="2" t="n"/>
     </row>
@@ -2365,15 +2365,15 @@
         <v>36</v>
       </c>
       <c r="E59" s="3" t="n">
-        <v>-46.71</v>
+        <v>-53.92</v>
       </c>
       <c r="F59" s="3" t="inlineStr">
         <is>
-          <t>15/42</t>
+          <t>12/42</t>
         </is>
       </c>
       <c r="G59" s="3" t="n">
-        <v>29.62</v>
+        <v>-525.14</v>
       </c>
       <c r="H59" s="3" t="n"/>
     </row>
@@ -2397,15 +2397,15 @@
         <v>10</v>
       </c>
       <c r="E60" s="2" t="n">
-        <v>65.17</v>
+        <v>33.25</v>
       </c>
       <c r="F60" s="2" t="inlineStr">
         <is>
-          <t>5/43</t>
+          <t>8/43</t>
         </is>
       </c>
       <c r="G60" s="2" t="n">
-        <v>94.79000000000001</v>
+        <v>-491.88</v>
       </c>
       <c r="H60" s="2" t="n"/>
     </row>
@@ -2429,15 +2429,15 @@
         <v>6</v>
       </c>
       <c r="E61" s="3" t="n">
-        <v>-27.89</v>
+        <v>-25.63</v>
       </c>
       <c r="F61" s="3" t="inlineStr">
         <is>
-          <t>29/42</t>
+          <t>23/42</t>
         </is>
       </c>
       <c r="G61" s="3" t="n">
-        <v>66.90000000000001</v>
+        <v>-517.51</v>
       </c>
       <c r="H61" s="3" t="n"/>
     </row>
@@ -2461,15 +2461,15 @@
         <v>2</v>
       </c>
       <c r="E62" s="2" t="n">
-        <v>6.6</v>
+        <v>-13.37</v>
       </c>
       <c r="F62" s="2" t="inlineStr">
         <is>
-          <t>41/43</t>
+          <t>22/43</t>
         </is>
       </c>
       <c r="G62" s="2" t="n">
-        <v>73.5</v>
+        <v>-530.89</v>
       </c>
       <c r="H62" s="2" t="n"/>
     </row>
@@ -2493,15 +2493,15 @@
         <v>6</v>
       </c>
       <c r="E63" s="3" t="n">
-        <v>-18.58</v>
+        <v>-16.41</v>
       </c>
       <c r="F63" s="3" t="inlineStr">
         <is>
-          <t>34/42</t>
+          <t>32/42</t>
         </is>
       </c>
       <c r="G63" s="3" t="n">
-        <v>54.92</v>
+        <v>-547.3</v>
       </c>
       <c r="H63" s="3" t="n"/>
     </row>
@@ -2525,15 +2525,15 @@
         <v>4</v>
       </c>
       <c r="E64" s="2" t="n">
-        <v>4.35</v>
+        <v>-3.04</v>
       </c>
       <c r="F64" s="2" t="inlineStr">
         <is>
-          <t>43/43</t>
+          <t>39/43</t>
         </is>
       </c>
       <c r="G64" s="2" t="n">
-        <v>59.26</v>
+        <v>-550.34</v>
       </c>
       <c r="H64" s="2" t="n"/>
     </row>
@@ -2557,15 +2557,15 @@
         <v>10</v>
       </c>
       <c r="E65" s="3" t="n">
-        <v>-15.62</v>
+        <v>-12.55</v>
       </c>
       <c r="F65" s="3" t="inlineStr">
         <is>
-          <t>38/42</t>
+          <t>36/42</t>
         </is>
       </c>
       <c r="G65" s="3" t="n">
-        <v>43.64</v>
+        <v>-562.89</v>
       </c>
       <c r="H65" s="3" t="n"/>
     </row>
@@ -2589,15 +2589,15 @@
         <v>4</v>
       </c>
       <c r="E66" s="2" t="n">
-        <v>18.52</v>
+        <v>-17.16</v>
       </c>
       <c r="F66" s="2" t="inlineStr">
         <is>
-          <t>26/43</t>
+          <t>20/43</t>
         </is>
       </c>
       <c r="G66" s="2" t="n">
-        <v>62.16</v>
+        <v>-580.05</v>
       </c>
       <c r="H66" s="2" t="n"/>
     </row>
@@ -2621,7 +2621,7 @@
         <v>20</v>
       </c>
       <c r="E67" s="3" t="n">
-        <v>-41.67</v>
+        <v>-44.9</v>
       </c>
       <c r="F67" s="3" t="inlineStr">
         <is>
@@ -2629,7 +2629,7 @@
         </is>
       </c>
       <c r="G67" s="3" t="n">
-        <v>20.49</v>
+        <v>-624.9400000000001</v>
       </c>
       <c r="H67" s="3" t="n"/>
     </row>
@@ -2653,15 +2653,15 @@
         <v>3</v>
       </c>
       <c r="E68" s="2" t="n">
-        <v>7.14</v>
+        <v>-4.93</v>
       </c>
       <c r="F68" s="2" t="inlineStr">
         <is>
-          <t>39/43</t>
+          <t>36/43</t>
         </is>
       </c>
       <c r="G68" s="2" t="n">
-        <v>27.63</v>
+        <v>-629.88</v>
       </c>
       <c r="H68" s="2" t="n"/>
     </row>
@@ -2685,15 +2685,15 @@
         <v>4</v>
       </c>
       <c r="E69" s="3" t="n">
-        <v>-11.67</v>
+        <v>-9.779999999999999</v>
       </c>
       <c r="F69" s="3" t="inlineStr">
         <is>
-          <t>42/42</t>
+          <t>38/42</t>
         </is>
       </c>
       <c r="G69" s="3" t="n">
-        <v>15.97</v>
+        <v>-639.66</v>
       </c>
       <c r="H69" s="3" t="n"/>
     </row>
@@ -2717,15 +2717,15 @@
         <v>17</v>
       </c>
       <c r="E70" s="2" t="n">
-        <v>160.38</v>
+        <v>54.35</v>
       </c>
       <c r="F70" s="2" t="inlineStr">
         <is>
-          <t>2/43</t>
+          <t>5/43</t>
         </is>
       </c>
       <c r="G70" s="2" t="n">
-        <v>176.34</v>
+        <v>-585.3099999999999</v>
       </c>
       <c r="H70" s="2" t="n"/>
     </row>
@@ -2749,15 +2749,15 @@
         <v>7</v>
       </c>
       <c r="E71" s="3" t="n">
-        <v>-67.39</v>
+        <v>-61.87</v>
       </c>
       <c r="F71" s="3" t="inlineStr">
         <is>
-          <t>3/42</t>
+          <t>9/42</t>
         </is>
       </c>
       <c r="G71" s="3" t="n">
-        <v>108.95</v>
+        <v>-647.1900000000001</v>
       </c>
       <c r="H71" s="3" t="n"/>
     </row>
@@ -2781,15 +2781,15 @@
         <v>8</v>
       </c>
       <c r="E72" s="2" t="n">
-        <v>23.33</v>
+        <v>1.51</v>
       </c>
       <c r="F72" s="2" t="inlineStr">
         <is>
-          <t>24/43</t>
+          <t>41/43</t>
         </is>
       </c>
       <c r="G72" s="2" t="n">
-        <v>132.29</v>
+        <v>-645.67</v>
       </c>
       <c r="H72" s="2" t="n"/>
     </row>
@@ -2813,15 +2813,15 @@
         <v>27</v>
       </c>
       <c r="E73" s="3" t="n">
-        <v>-39.46</v>
+        <v>-18.65</v>
       </c>
       <c r="F73" s="3" t="inlineStr">
         <is>
-          <t>20/42</t>
+          <t>29/42</t>
         </is>
       </c>
       <c r="G73" s="3" t="n">
-        <v>92.83</v>
+        <v>-664.3200000000001</v>
       </c>
       <c r="H73" s="3" t="n"/>
     </row>
@@ -2845,15 +2845,15 @@
         <v>5</v>
       </c>
       <c r="E74" s="2" t="n">
-        <v>59.52</v>
+        <v>45.03</v>
       </c>
       <c r="F74" s="2" t="inlineStr">
         <is>
-          <t>7/43</t>
+          <t>6/43</t>
         </is>
       </c>
       <c r="G74" s="2" t="n">
-        <v>152.35</v>
+        <v>-619.29</v>
       </c>
       <c r="H74" s="2" t="n"/>
     </row>
@@ -2877,15 +2877,15 @@
         <v>34</v>
       </c>
       <c r="E75" s="3" t="n">
-        <v>-61.19</v>
+        <v>-73.95</v>
       </c>
       <c r="F75" s="3" t="inlineStr">
         <is>
-          <t>6/42</t>
+          <t>3/42</t>
         </is>
       </c>
       <c r="G75" s="3" t="n">
-        <v>91.16</v>
+        <v>-693.24</v>
       </c>
       <c r="H75" s="3" t="n"/>
     </row>
@@ -2909,15 +2909,15 @@
         <v>2</v>
       </c>
       <c r="E76" s="2" t="n">
-        <v>27.03</v>
+        <v>12.66</v>
       </c>
       <c r="F76" s="2" t="inlineStr">
         <is>
-          <t>21/43</t>
+          <t>24/43</t>
         </is>
       </c>
       <c r="G76" s="2" t="n">
-        <v>118.18</v>
+        <v>-680.58</v>
       </c>
       <c r="H76" s="2" t="n"/>
     </row>
@@ -2941,15 +2941,15 @@
         <v>19</v>
       </c>
       <c r="E77" s="3" t="n">
-        <v>-47.52</v>
+        <v>-54.22</v>
       </c>
       <c r="F77" s="3" t="inlineStr">
         <is>
-          <t>14/42</t>
+          <t>11/42</t>
         </is>
       </c>
       <c r="G77" s="3" t="n">
-        <v>70.67</v>
+        <v>-734.8099999999999</v>
       </c>
       <c r="H77" s="3" t="n"/>
     </row>
@@ -2973,15 +2973,15 @@
         <v>2</v>
       </c>
       <c r="E78" s="2" t="n">
-        <v>5.46</v>
+        <v>-20.38</v>
       </c>
       <c r="F78" s="2" t="inlineStr">
         <is>
-          <t>42/43</t>
+          <t>18/43</t>
         </is>
       </c>
       <c r="G78" s="2" t="n">
-        <v>76.13</v>
+        <v>-755.1799999999999</v>
       </c>
       <c r="H78" s="2" t="n"/>
     </row>
@@ -3005,7 +3005,7 @@
         <v>18</v>
       </c>
       <c r="E79" s="3" t="n">
-        <v>-41.18</v>
+        <v>-41.13</v>
       </c>
       <c r="F79" s="3" t="inlineStr">
         <is>
@@ -3013,7 +3013,7 @@
         </is>
       </c>
       <c r="G79" s="3" t="n">
-        <v>34.94</v>
+        <v>-796.3099999999999</v>
       </c>
       <c r="H79" s="3" t="n"/>
     </row>
@@ -3037,15 +3037,15 @@
         <v>2</v>
       </c>
       <c r="E80" s="2" t="n">
-        <v>15.72</v>
+        <v>8.09</v>
       </c>
       <c r="F80" s="2" t="inlineStr">
         <is>
-          <t>29/43</t>
+          <t>31/43</t>
         </is>
       </c>
       <c r="G80" s="2" t="n">
-        <v>50.67</v>
+        <v>-788.22</v>
       </c>
       <c r="H80" s="2" t="n"/>
     </row>
@@ -3069,15 +3069,15 @@
         <v>33</v>
       </c>
       <c r="E81" s="3" t="n">
-        <v>-50.72</v>
+        <v>-48.57</v>
       </c>
       <c r="F81" s="3" t="inlineStr">
         <is>
-          <t>13/42</t>
+          <t>15/42</t>
         </is>
       </c>
       <c r="G81" s="3" t="n">
-        <v>-0.06</v>
+        <v>-836.79</v>
       </c>
       <c r="H81" s="3" t="n"/>
     </row>
@@ -3101,15 +3101,15 @@
         <v>5</v>
       </c>
       <c r="E82" s="2" t="n">
-        <v>14.34</v>
+        <v>-3.89</v>
       </c>
       <c r="F82" s="2" t="inlineStr">
         <is>
-          <t>31/43</t>
+          <t>37/43</t>
         </is>
       </c>
       <c r="G82" s="2" t="n">
-        <v>14.28</v>
+        <v>-840.6799999999999</v>
       </c>
       <c r="H82" s="2" t="n"/>
     </row>
@@ -3133,15 +3133,15 @@
         <v>10</v>
       </c>
       <c r="E83" s="3" t="n">
-        <v>-33.44</v>
+        <v>-23.43</v>
       </c>
       <c r="F83" s="3" t="inlineStr">
         <is>
-          <t>22/42</t>
+          <t>26/42</t>
         </is>
       </c>
       <c r="G83" s="3" t="n">
-        <v>-19.16</v>
+        <v>-864.11</v>
       </c>
       <c r="H83" s="3" t="n"/>
     </row>
@@ -3165,15 +3165,15 @@
         <v>4</v>
       </c>
       <c r="E84" s="2" t="n">
-        <v>63</v>
+        <v>28.64</v>
       </c>
       <c r="F84" s="2" t="inlineStr">
         <is>
-          <t>6/43</t>
+          <t>12/43</t>
         </is>
       </c>
       <c r="G84" s="2" t="n">
-        <v>43.84</v>
+        <v>-835.47</v>
       </c>
       <c r="H84" s="2" t="n"/>
     </row>
@@ -3197,15 +3197,15 @@
         <v>29</v>
       </c>
       <c r="E85" s="3" t="n">
-        <v>-75.68000000000001</v>
+        <v>-49.5</v>
       </c>
       <c r="F85" s="3" t="inlineStr">
         <is>
-          <t>2/42</t>
+          <t>13/42</t>
         </is>
       </c>
       <c r="G85" s="3" t="n">
-        <v>-31.84</v>
+        <v>-884.96</v>
       </c>
       <c r="H85" s="3" t="n"/>
     </row>
@@ -3229,15 +3229,15 @@
         <v>4</v>
       </c>
       <c r="E86" s="2" t="n">
-        <v>39.13</v>
+        <v>-2.56</v>
       </c>
       <c r="F86" s="2" t="inlineStr">
         <is>
-          <t>14/43</t>
+          <t>40/43</t>
         </is>
       </c>
       <c r="G86" s="2" t="n">
-        <v>7.29</v>
+        <v>-887.52</v>
       </c>
       <c r="H86" s="2" t="n"/>
     </row>

</xml_diff>